<commit_message>
add abundance by location
</commit_message>
<xml_diff>
--- a/expt1and2metadata.xlsx
+++ b/expt1and2metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24680" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24640" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="210">
   <si>
     <t>1-t0-poop</t>
   </si>
@@ -597,27 +597,12 @@
     <t>colon</t>
   </si>
   <si>
-    <t>colcon2</t>
-  </si>
-  <si>
-    <t>colon2</t>
-  </si>
-  <si>
     <t>spleen</t>
   </si>
   <si>
-    <t>cec</t>
-  </si>
-  <si>
     <t>t</t>
   </si>
   <si>
-    <t>colocon</t>
-  </si>
-  <si>
-    <t>stool</t>
-  </si>
-  <si>
     <t>sampleID</t>
   </si>
   <si>
@@ -649,9 +634,6 @@
   </si>
   <si>
     <t>D</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> FALSE</t>
   </si>
   <si>
     <t>E</t>
@@ -722,8 +704,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -760,7 +754,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="41">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -775,6 +769,12 @@
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -789,6 +789,12 @@
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1118,10 +1124,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H193"/>
+  <dimension ref="A1:K193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="A91" sqref="A1:H91"/>
+    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="A92" sqref="A92:H187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1131,28 +1137,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>205</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1163,7 +1169,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1178,7 +1184,7 @@
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1189,7 +1195,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D3">
         <v>24</v>
@@ -1204,7 +1210,7 @@
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1215,7 +1221,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -1230,7 +1236,7 @@
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1241,7 +1247,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D5">
         <v>48</v>
@@ -1256,7 +1262,7 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1267,7 +1273,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D6">
         <v>48</v>
@@ -1282,7 +1288,7 @@
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1293,7 +1299,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D7">
         <v>48</v>
@@ -1308,7 +1314,7 @@
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1319,7 +1325,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D8">
         <v>48</v>
@@ -1334,7 +1340,7 @@
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1345,7 +1351,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1360,7 +1366,7 @@
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1371,7 +1377,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D10">
         <v>24</v>
@@ -1386,7 +1392,7 @@
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1397,7 +1403,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D11">
         <v>3</v>
@@ -1412,7 +1418,7 @@
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1423,7 +1429,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D12">
         <v>48</v>
@@ -1438,7 +1444,7 @@
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1449,7 +1455,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D13">
         <v>48</v>
@@ -1464,7 +1470,7 @@
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1475,7 +1481,7 @@
         <v>3</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -1490,7 +1496,7 @@
         <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1501,7 +1507,7 @@
         <v>3</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D15">
         <v>24</v>
@@ -1516,7 +1522,7 @@
         <v>0</v>
       </c>
       <c r="H15" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1527,7 +1533,7 @@
         <v>3</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D16">
         <v>3</v>
@@ -1542,7 +1548,7 @@
         <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1553,7 +1559,7 @@
         <v>3</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D17">
         <v>48</v>
@@ -1568,7 +1574,7 @@
         <v>0</v>
       </c>
       <c r="H17" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1579,7 +1585,7 @@
         <v>3</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D18">
         <v>48</v>
@@ -1594,7 +1600,7 @@
         <v>0</v>
       </c>
       <c r="H18" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -1605,7 +1611,7 @@
         <v>3</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D19">
         <v>48</v>
@@ -1620,7 +1626,7 @@
         <v>0</v>
       </c>
       <c r="H19" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1631,7 +1637,7 @@
         <v>3</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D20">
         <v>48</v>
@@ -1646,7 +1652,7 @@
         <v>0</v>
       </c>
       <c r="H20" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1657,7 +1663,7 @@
         <v>4</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -1672,7 +1678,7 @@
         <v>0</v>
       </c>
       <c r="H21" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1683,7 +1689,7 @@
         <v>4</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D22">
         <v>24</v>
@@ -1698,7 +1704,7 @@
         <v>0</v>
       </c>
       <c r="H22" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1709,7 +1715,7 @@
         <v>4</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D23">
         <v>3</v>
@@ -1724,7 +1730,7 @@
         <v>0</v>
       </c>
       <c r="H23" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1735,7 +1741,7 @@
         <v>4</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D24">
         <v>48</v>
@@ -1750,7 +1756,7 @@
         <v>0</v>
       </c>
       <c r="H24" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1761,7 +1767,7 @@
         <v>4</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D25">
         <v>48</v>
@@ -1776,7 +1782,7 @@
         <v>0</v>
       </c>
       <c r="H25" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1787,7 +1793,7 @@
         <v>4</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D26">
         <v>48</v>
@@ -1802,7 +1808,7 @@
         <v>0</v>
       </c>
       <c r="H26" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1813,7 +1819,7 @@
         <v>4</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D27">
         <v>48</v>
@@ -1828,7 +1834,7 @@
         <v>0</v>
       </c>
       <c r="H27" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1839,7 +1845,7 @@
         <v>5</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -1854,7 +1860,7 @@
         <v>1</v>
       </c>
       <c r="H28" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1865,7 +1871,7 @@
         <v>5</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D29">
         <v>24</v>
@@ -1880,7 +1886,7 @@
         <v>1</v>
       </c>
       <c r="H29" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1891,7 +1897,7 @@
         <v>5</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D30">
         <v>3</v>
@@ -1906,7 +1912,7 @@
         <v>1</v>
       </c>
       <c r="H30" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1917,7 +1923,7 @@
         <v>5</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D31">
         <v>48</v>
@@ -1932,7 +1938,7 @@
         <v>1</v>
       </c>
       <c r="H31" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1943,7 +1949,7 @@
         <v>5</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D32">
         <v>48</v>
@@ -1958,7 +1964,7 @@
         <v>1</v>
       </c>
       <c r="H32" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1969,7 +1975,7 @@
         <v>5</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D33">
         <v>48</v>
@@ -1984,7 +1990,7 @@
         <v>1</v>
       </c>
       <c r="H33" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1995,7 +2001,7 @@
         <v>6</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -2010,7 +2016,7 @@
         <v>1</v>
       </c>
       <c r="H34" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -2021,7 +2027,7 @@
         <v>6</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D35">
         <v>24</v>
@@ -2036,7 +2042,7 @@
         <v>1</v>
       </c>
       <c r="H35" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -2047,7 +2053,7 @@
         <v>6</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D36">
         <v>3</v>
@@ -2062,7 +2068,7 @@
         <v>1</v>
       </c>
       <c r="H36" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -2073,7 +2079,7 @@
         <v>6</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D37">
         <v>48</v>
@@ -2088,7 +2094,7 @@
         <v>1</v>
       </c>
       <c r="H37" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -2099,7 +2105,7 @@
         <v>6</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D38">
         <v>48</v>
@@ -2114,7 +2120,7 @@
         <v>1</v>
       </c>
       <c r="H38" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -2125,7 +2131,7 @@
         <v>6</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D39">
         <v>48</v>
@@ -2140,7 +2146,7 @@
         <v>1</v>
       </c>
       <c r="H39" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -2151,7 +2157,7 @@
         <v>7</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -2166,7 +2172,7 @@
         <v>1</v>
       </c>
       <c r="H40" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -2177,7 +2183,7 @@
         <v>7</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D41">
         <v>24</v>
@@ -2192,7 +2198,7 @@
         <v>1</v>
       </c>
       <c r="H41" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -2203,7 +2209,7 @@
         <v>7</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D42">
         <v>3</v>
@@ -2218,7 +2224,7 @@
         <v>1</v>
       </c>
       <c r="H42" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -2229,7 +2235,7 @@
         <v>7</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D43">
         <v>48</v>
@@ -2244,7 +2250,7 @@
         <v>1</v>
       </c>
       <c r="H43" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -2255,7 +2261,7 @@
         <v>7</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D44">
         <v>48</v>
@@ -2270,7 +2276,7 @@
         <v>1</v>
       </c>
       <c r="H44" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -2281,7 +2287,7 @@
         <v>7</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D45">
         <v>48</v>
@@ -2296,7 +2302,7 @@
         <v>1</v>
       </c>
       <c r="H45" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -2307,7 +2313,7 @@
         <v>8</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D46">
         <v>0</v>
@@ -2322,7 +2328,7 @@
         <v>1</v>
       </c>
       <c r="H46" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -2333,7 +2339,7 @@
         <v>8</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D47">
         <v>24</v>
@@ -2348,7 +2354,7 @@
         <v>1</v>
       </c>
       <c r="H47" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -2359,7 +2365,7 @@
         <v>8</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D48">
         <v>48</v>
@@ -2374,7 +2380,7 @@
         <v>1</v>
       </c>
       <c r="H48" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -2385,7 +2391,7 @@
         <v>8</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D49">
         <v>48</v>
@@ -2400,7 +2406,7 @@
         <v>1</v>
       </c>
       <c r="H49" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -2411,7 +2417,7 @@
         <v>8</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D50">
         <v>48</v>
@@ -2426,7 +2432,7 @@
         <v>1</v>
       </c>
       <c r="H50" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -2437,7 +2443,7 @@
         <v>9</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D51">
         <v>0</v>
@@ -2452,7 +2458,7 @@
         <v>1</v>
       </c>
       <c r="H51" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -2463,7 +2469,7 @@
         <v>9</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D52">
         <v>24</v>
@@ -2478,7 +2484,7 @@
         <v>1</v>
       </c>
       <c r="H52" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -2489,7 +2495,7 @@
         <v>9</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D53">
         <v>3</v>
@@ -2504,7 +2510,7 @@
         <v>1</v>
       </c>
       <c r="H53" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -2515,7 +2521,7 @@
         <v>9</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D54">
         <v>48</v>
@@ -2530,7 +2536,7 @@
         <v>1</v>
       </c>
       <c r="H54" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -2541,7 +2547,7 @@
         <v>9</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D55">
         <v>48</v>
@@ -2556,7 +2562,7 @@
         <v>1</v>
       </c>
       <c r="H55" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -2567,7 +2573,7 @@
         <v>9</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D56">
         <v>48</v>
@@ -2582,7 +2588,7 @@
         <v>1</v>
       </c>
       <c r="H56" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -2593,7 +2599,7 @@
         <v>9</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D57">
         <v>48</v>
@@ -2608,7 +2614,7 @@
         <v>1</v>
       </c>
       <c r="H57" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -2619,7 +2625,7 @@
         <v>10</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D58">
         <v>0</v>
@@ -2634,7 +2640,7 @@
         <v>1</v>
       </c>
       <c r="H58" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -2645,7 +2651,7 @@
         <v>10</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D59">
         <v>24</v>
@@ -2660,7 +2666,7 @@
         <v>1</v>
       </c>
       <c r="H59" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -2671,7 +2677,7 @@
         <v>10</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D60">
         <v>3</v>
@@ -2686,7 +2692,7 @@
         <v>1</v>
       </c>
       <c r="H60" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -2697,7 +2703,7 @@
         <v>10</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D61">
         <v>48</v>
@@ -2712,7 +2718,7 @@
         <v>1</v>
       </c>
       <c r="H61" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -2723,7 +2729,7 @@
         <v>10</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D62">
         <v>48</v>
@@ -2738,7 +2744,7 @@
         <v>1</v>
       </c>
       <c r="H62" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -2749,7 +2755,7 @@
         <v>10</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D63">
         <v>48</v>
@@ -2764,7 +2770,7 @@
         <v>1</v>
       </c>
       <c r="H63" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -2775,7 +2781,7 @@
         <v>10</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D64">
         <v>48</v>
@@ -2790,7 +2796,7 @@
         <v>1</v>
       </c>
       <c r="H64" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -2801,7 +2807,7 @@
         <v>11</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D65">
         <v>0</v>
@@ -2816,7 +2822,7 @@
         <v>1</v>
       </c>
       <c r="H65" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -2827,7 +2833,7 @@
         <v>11</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D66">
         <v>24</v>
@@ -2842,7 +2848,7 @@
         <v>1</v>
       </c>
       <c r="H66" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -2853,7 +2859,7 @@
         <v>11</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D67">
         <v>3</v>
@@ -2868,7 +2874,7 @@
         <v>1</v>
       </c>
       <c r="H67" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -2879,7 +2885,7 @@
         <v>11</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D68">
         <v>48</v>
@@ -2894,7 +2900,7 @@
         <v>1</v>
       </c>
       <c r="H68" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -2905,7 +2911,7 @@
         <v>11</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D69">
         <v>48</v>
@@ -2920,7 +2926,7 @@
         <v>1</v>
       </c>
       <c r="H69" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -2931,7 +2937,7 @@
         <v>11</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D70">
         <v>48</v>
@@ -2946,7 +2952,7 @@
         <v>1</v>
       </c>
       <c r="H70" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -2957,7 +2963,7 @@
         <v>11</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D71">
         <v>48</v>
@@ -2972,7 +2978,7 @@
         <v>1</v>
       </c>
       <c r="H71" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -2983,7 +2989,7 @@
         <v>12</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D72">
         <v>0</v>
@@ -2998,7 +3004,7 @@
         <v>1</v>
       </c>
       <c r="H72" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -3009,7 +3015,7 @@
         <v>12</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D73">
         <v>24</v>
@@ -3024,7 +3030,7 @@
         <v>1</v>
       </c>
       <c r="H73" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -3035,7 +3041,7 @@
         <v>12</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D74">
         <v>3</v>
@@ -3050,7 +3056,7 @@
         <v>1</v>
       </c>
       <c r="H74" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -3061,7 +3067,7 @@
         <v>12</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D75">
         <v>48</v>
@@ -3076,7 +3082,7 @@
         <v>1</v>
       </c>
       <c r="H75" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -3087,7 +3093,7 @@
         <v>12</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D76">
         <v>48</v>
@@ -3102,7 +3108,7 @@
         <v>1</v>
       </c>
       <c r="H76" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -3113,7 +3119,7 @@
         <v>12</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D77">
         <v>48</v>
@@ -3128,7 +3134,7 @@
         <v>1</v>
       </c>
       <c r="H77" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -3139,7 +3145,7 @@
         <v>12</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D78">
         <v>48</v>
@@ -3154,7 +3160,7 @@
         <v>1</v>
       </c>
       <c r="H78" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -3165,7 +3171,7 @@
         <v>13</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D79">
         <v>0</v>
@@ -3180,7 +3186,7 @@
         <v>1</v>
       </c>
       <c r="H79" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -3191,7 +3197,7 @@
         <v>13</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D80">
         <v>24</v>
@@ -3206,10 +3212,10 @@
         <v>1</v>
       </c>
       <c r="H80" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11">
       <c r="A81" t="s">
         <v>58</v>
       </c>
@@ -3217,7 +3223,7 @@
         <v>13</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D81">
         <v>3</v>
@@ -3232,10 +3238,10 @@
         <v>1</v>
       </c>
       <c r="H81" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11">
       <c r="A82" t="s">
         <v>62</v>
       </c>
@@ -3243,7 +3249,7 @@
         <v>13</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D82">
         <v>48</v>
@@ -3258,10 +3264,10 @@
         <v>1</v>
       </c>
       <c r="H82" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11">
       <c r="A83" t="s">
         <v>63</v>
       </c>
@@ -3269,7 +3275,7 @@
         <v>13</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D83">
         <v>48</v>
@@ -3284,10 +3290,10 @@
         <v>1</v>
       </c>
       <c r="H83" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11">
       <c r="A84" t="s">
         <v>64</v>
       </c>
@@ -3295,7 +3301,7 @@
         <v>13</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D84">
         <v>48</v>
@@ -3310,10 +3316,10 @@
         <v>1</v>
       </c>
       <c r="H84" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11">
       <c r="A85" t="s">
         <v>65</v>
       </c>
@@ -3321,7 +3327,7 @@
         <v>13</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D85">
         <v>48</v>
@@ -3336,10 +3342,10 @@
         <v>1</v>
       </c>
       <c r="H85" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11">
       <c r="A86" t="s">
         <v>66</v>
       </c>
@@ -3347,7 +3353,7 @@
         <v>14</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D86">
         <v>0</v>
@@ -3362,10 +3368,10 @@
         <v>1</v>
       </c>
       <c r="H86" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11">
       <c r="A87" t="s">
         <v>68</v>
       </c>
@@ -3373,7 +3379,7 @@
         <v>14</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D87">
         <v>24</v>
@@ -3388,10 +3394,10 @@
         <v>1</v>
       </c>
       <c r="H87" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11">
       <c r="A88" t="s">
         <v>70</v>
       </c>
@@ -3399,7 +3405,7 @@
         <v>14</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D88">
         <v>48</v>
@@ -3414,10 +3420,10 @@
         <v>1</v>
       </c>
       <c r="H88" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11">
       <c r="A89" t="s">
         <v>72</v>
       </c>
@@ -3425,7 +3431,7 @@
         <v>14</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D89">
         <v>48</v>
@@ -3440,10 +3446,10 @@
         <v>1</v>
       </c>
       <c r="H89" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11">
       <c r="A90" t="s">
         <v>74</v>
       </c>
@@ -3451,7 +3457,7 @@
         <v>14</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D90">
         <v>48</v>
@@ -3466,10 +3472,10 @@
         <v>1</v>
       </c>
       <c r="H90" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11">
       <c r="A91" t="s">
         <v>76</v>
       </c>
@@ -3477,7 +3483,7 @@
         <v>14</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D91">
         <v>48</v>
@@ -3492,10 +3498,10 @@
         <v>1</v>
       </c>
       <c r="H91" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11">
       <c r="A92" t="s">
         <v>1</v>
       </c>
@@ -3503,7 +3509,7 @@
         <v>1</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D92">
         <v>0</v>
@@ -3514,14 +3520,14 @@
       <c r="F92">
         <v>2</v>
       </c>
-      <c r="G92" t="s">
-        <v>210</v>
+      <c r="G92" t="b">
+        <v>0</v>
       </c>
       <c r="H92" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11">
       <c r="A93" t="s">
         <v>3</v>
       </c>
@@ -3529,7 +3535,7 @@
         <v>1</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D93">
         <v>24</v>
@@ -3540,14 +3546,14 @@
       <c r="F93">
         <v>2</v>
       </c>
-      <c r="G93" t="s">
-        <v>210</v>
+      <c r="G93" t="b">
+        <v>0</v>
       </c>
       <c r="H93" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11">
       <c r="A94" t="s">
         <v>5</v>
       </c>
@@ -3555,7 +3561,7 @@
         <v>1</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D94">
         <v>3</v>
@@ -3566,14 +3572,17 @@
       <c r="F94">
         <v>2</v>
       </c>
-      <c r="G94" t="s">
-        <v>210</v>
+      <c r="G94" t="b">
+        <v>0</v>
       </c>
       <c r="H94" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8">
+        <v>209</v>
+      </c>
+      <c r="K94" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11">
       <c r="A95" t="s">
         <v>10</v>
       </c>
@@ -3581,7 +3590,7 @@
         <v>1</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D95">
         <v>48</v>
@@ -3592,14 +3601,17 @@
       <c r="F95">
         <v>2</v>
       </c>
-      <c r="G95" t="s">
-        <v>210</v>
+      <c r="G95" t="b">
+        <v>0</v>
       </c>
       <c r="H95" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8">
+        <v>209</v>
+      </c>
+      <c r="K95" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11">
       <c r="A96" t="s">
         <v>11</v>
       </c>
@@ -3607,7 +3619,7 @@
         <v>1</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D96">
         <v>96</v>
@@ -3618,14 +3630,17 @@
       <c r="F96">
         <v>2</v>
       </c>
-      <c r="G96" t="s">
-        <v>210</v>
+      <c r="G96" t="b">
+        <v>0</v>
       </c>
       <c r="H96" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8">
+        <v>209</v>
+      </c>
+      <c r="K96" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11">
       <c r="A97" t="s">
         <v>12</v>
       </c>
@@ -3633,7 +3648,7 @@
         <v>1</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D97">
         <v>96</v>
@@ -3644,14 +3659,17 @@
       <c r="F97">
         <v>2</v>
       </c>
-      <c r="G97" t="s">
-        <v>210</v>
+      <c r="G97" t="b">
+        <v>0</v>
       </c>
       <c r="H97" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8">
+        <v>209</v>
+      </c>
+      <c r="K97" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11">
       <c r="A98" t="s">
         <v>13</v>
       </c>
@@ -3659,7 +3677,7 @@
         <v>1</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D98">
         <v>96</v>
@@ -3670,14 +3688,17 @@
       <c r="F98">
         <v>2</v>
       </c>
-      <c r="G98" t="s">
-        <v>210</v>
+      <c r="G98" t="b">
+        <v>0</v>
       </c>
       <c r="H98" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8">
+        <v>209</v>
+      </c>
+      <c r="K98" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11">
       <c r="A99" t="s">
         <v>88</v>
       </c>
@@ -3685,7 +3706,7 @@
         <v>2</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D99">
         <v>96</v>
@@ -3696,14 +3717,17 @@
       <c r="F99">
         <v>2</v>
       </c>
-      <c r="G99" t="s">
-        <v>210</v>
+      <c r="G99" t="b">
+        <v>0</v>
       </c>
       <c r="H99" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8">
+        <v>209</v>
+      </c>
+      <c r="K99" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11">
       <c r="A100" t="s">
         <v>89</v>
       </c>
@@ -3711,25 +3735,28 @@
         <v>2</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D100">
         <v>96</v>
       </c>
       <c r="E100" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F100">
         <v>2</v>
       </c>
-      <c r="G100" t="s">
-        <v>210</v>
+      <c r="G100" t="b">
+        <v>0</v>
       </c>
       <c r="H100" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8">
+        <v>209</v>
+      </c>
+      <c r="K100" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11">
       <c r="A101" t="s">
         <v>79</v>
       </c>
@@ -3737,7 +3764,7 @@
         <v>2</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D101">
         <v>0</v>
@@ -3748,14 +3775,17 @@
       <c r="F101">
         <v>2</v>
       </c>
-      <c r="G101" t="s">
-        <v>210</v>
+      <c r="G101" t="b">
+        <v>0</v>
       </c>
       <c r="H101" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8">
+        <v>209</v>
+      </c>
+      <c r="K101" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11">
       <c r="A102" t="s">
         <v>81</v>
       </c>
@@ -3763,7 +3793,7 @@
         <v>2</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D102">
         <v>24</v>
@@ -3774,14 +3804,17 @@
       <c r="F102">
         <v>2</v>
       </c>
-      <c r="G102" t="s">
-        <v>210</v>
+      <c r="G102" t="b">
+        <v>0</v>
       </c>
       <c r="H102" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8">
+        <v>209</v>
+      </c>
+      <c r="K102" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11">
       <c r="A103" t="s">
         <v>83</v>
       </c>
@@ -3789,7 +3822,7 @@
         <v>2</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D103">
         <v>3</v>
@@ -3800,14 +3833,17 @@
       <c r="F103">
         <v>2</v>
       </c>
-      <c r="G103" t="s">
-        <v>210</v>
+      <c r="G103" t="b">
+        <v>0</v>
       </c>
       <c r="H103" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8">
+        <v>209</v>
+      </c>
+      <c r="K103" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11">
       <c r="A104" t="s">
         <v>86</v>
       </c>
@@ -3815,7 +3851,7 @@
         <v>2</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D104">
         <v>48</v>
@@ -3826,14 +3862,17 @@
       <c r="F104">
         <v>2</v>
       </c>
-      <c r="G104" t="s">
-        <v>210</v>
+      <c r="G104" t="b">
+        <v>0</v>
       </c>
       <c r="H104" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8">
+        <v>209</v>
+      </c>
+      <c r="K104" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11">
       <c r="A105" t="s">
         <v>87</v>
       </c>
@@ -3841,7 +3880,7 @@
         <v>2</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D105">
         <v>72</v>
@@ -3852,14 +3891,17 @@
       <c r="F105">
         <v>2</v>
       </c>
-      <c r="G105" t="s">
-        <v>210</v>
+      <c r="G105" t="b">
+        <v>0</v>
       </c>
       <c r="H105" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8">
+        <v>209</v>
+      </c>
+      <c r="K105" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11">
       <c r="A106" t="s">
         <v>90</v>
       </c>
@@ -3867,25 +3909,28 @@
         <v>2</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D106">
         <v>96</v>
       </c>
       <c r="E106" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F106">
         <v>2</v>
       </c>
-      <c r="G106" t="s">
-        <v>210</v>
+      <c r="G106" t="b">
+        <v>0</v>
       </c>
       <c r="H106" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8">
+        <v>209</v>
+      </c>
+      <c r="K106" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11">
       <c r="A107" t="s">
         <v>93</v>
       </c>
@@ -3893,7 +3938,7 @@
         <v>3</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D107">
         <v>24</v>
@@ -3904,14 +3949,17 @@
       <c r="F107">
         <v>2</v>
       </c>
-      <c r="G107" t="s">
-        <v>210</v>
+      <c r="G107" t="b">
+        <v>0</v>
       </c>
       <c r="H107" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8">
+        <v>209</v>
+      </c>
+      <c r="K107" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11">
       <c r="A108" t="s">
         <v>95</v>
       </c>
@@ -3919,7 +3967,7 @@
         <v>3</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D108">
         <v>3</v>
@@ -3930,14 +3978,17 @@
       <c r="F108">
         <v>2</v>
       </c>
-      <c r="G108" t="s">
-        <v>210</v>
+      <c r="G108" t="b">
+        <v>0</v>
       </c>
       <c r="H108" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8">
+        <v>209</v>
+      </c>
+      <c r="K108" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11">
       <c r="A109" t="s">
         <v>97</v>
       </c>
@@ -3945,7 +3996,7 @@
         <v>3</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D109">
         <v>48</v>
@@ -3956,14 +4007,17 @@
       <c r="F109">
         <v>2</v>
       </c>
-      <c r="G109" t="s">
-        <v>210</v>
+      <c r="G109" t="b">
+        <v>0</v>
       </c>
       <c r="H109" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8">
+        <v>209</v>
+      </c>
+      <c r="K109" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11">
       <c r="A110" t="s">
         <v>99</v>
       </c>
@@ -3971,7 +4025,7 @@
         <v>3</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D110">
         <v>48</v>
@@ -3982,14 +4036,17 @@
       <c r="F110">
         <v>2</v>
       </c>
-      <c r="G110" t="s">
-        <v>210</v>
+      <c r="G110" t="b">
+        <v>0</v>
       </c>
       <c r="H110" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8">
+        <v>209</v>
+      </c>
+      <c r="K110" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11">
       <c r="A111" t="s">
         <v>101</v>
       </c>
@@ -3997,7 +4054,7 @@
         <v>3</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D111">
         <v>48</v>
@@ -4008,14 +4065,17 @@
       <c r="F111">
         <v>2</v>
       </c>
-      <c r="G111" t="s">
-        <v>210</v>
+      <c r="G111" t="b">
+        <v>0</v>
       </c>
       <c r="H111" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8">
+        <v>209</v>
+      </c>
+      <c r="K111" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11">
       <c r="A112" t="s">
         <v>115</v>
       </c>
@@ -4023,7 +4083,7 @@
         <v>4</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D112">
         <v>96</v>
@@ -4038,10 +4098,13 @@
         <v>1</v>
       </c>
       <c r="H112" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8">
+        <v>206</v>
+      </c>
+      <c r="K112" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11">
       <c r="A113" t="s">
         <v>116</v>
       </c>
@@ -4049,7 +4112,7 @@
         <v>4</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D113">
         <v>96</v>
@@ -4064,10 +4127,13 @@
         <v>1</v>
       </c>
       <c r="H113" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8">
+        <v>206</v>
+      </c>
+      <c r="K113" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11">
       <c r="A114" t="s">
         <v>104</v>
       </c>
@@ -4075,7 +4141,7 @@
         <v>4</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D114">
         <v>0</v>
@@ -4090,10 +4156,13 @@
         <v>1</v>
       </c>
       <c r="H114" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8">
+        <v>206</v>
+      </c>
+      <c r="K114" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11">
       <c r="A115" t="s">
         <v>106</v>
       </c>
@@ -4101,7 +4170,7 @@
         <v>4</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D115">
         <v>24</v>
@@ -4116,10 +4185,13 @@
         <v>1</v>
       </c>
       <c r="H115" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8">
+        <v>206</v>
+      </c>
+      <c r="K115" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11">
       <c r="A116" t="s">
         <v>108</v>
       </c>
@@ -4127,7 +4199,7 @@
         <v>4</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D116">
         <v>3</v>
@@ -4142,10 +4214,13 @@
         <v>1</v>
       </c>
       <c r="H116" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8">
+        <v>206</v>
+      </c>
+      <c r="K116" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11">
       <c r="A117" t="s">
         <v>113</v>
       </c>
@@ -4153,7 +4228,7 @@
         <v>4</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D117">
         <v>48</v>
@@ -4168,10 +4243,13 @@
         <v>1</v>
       </c>
       <c r="H117" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8">
+        <v>206</v>
+      </c>
+      <c r="K117" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11">
       <c r="A118" t="s">
         <v>114</v>
       </c>
@@ -4179,7 +4257,7 @@
         <v>4</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D118">
         <v>72</v>
@@ -4194,10 +4272,13 @@
         <v>1</v>
       </c>
       <c r="H118" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8">
+        <v>206</v>
+      </c>
+      <c r="K118" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11">
       <c r="A119" t="s">
         <v>117</v>
       </c>
@@ -4205,13 +4286,13 @@
         <v>4</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D119">
         <v>96</v>
       </c>
       <c r="E119" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F119">
         <v>2</v>
@@ -4220,10 +4301,13 @@
         <v>1</v>
       </c>
       <c r="H119" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8">
+        <v>206</v>
+      </c>
+      <c r="K119" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11">
       <c r="A120" t="s">
         <v>118</v>
       </c>
@@ -4231,13 +4315,13 @@
         <v>5</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D120">
         <v>48</v>
       </c>
       <c r="E120" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="F120">
         <v>2</v>
@@ -4246,10 +4330,10 @@
         <v>1</v>
       </c>
       <c r="H120" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11">
       <c r="A121" t="s">
         <v>120</v>
       </c>
@@ -4257,7 +4341,7 @@
         <v>5</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D121">
         <v>0</v>
@@ -4272,10 +4356,10 @@
         <v>1</v>
       </c>
       <c r="H121" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11">
       <c r="A122" t="s">
         <v>122</v>
       </c>
@@ -4283,7 +4367,7 @@
         <v>5</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D122">
         <v>24</v>
@@ -4298,10 +4382,10 @@
         <v>1</v>
       </c>
       <c r="H122" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11">
       <c r="A123" t="s">
         <v>124</v>
       </c>
@@ -4309,7 +4393,7 @@
         <v>5</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D123">
         <v>3</v>
@@ -4324,10 +4408,10 @@
         <v>1</v>
       </c>
       <c r="H123" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11">
       <c r="A124" t="s">
         <v>128</v>
       </c>
@@ -4335,7 +4419,7 @@
         <v>5</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D124">
         <v>48</v>
@@ -4350,10 +4434,10 @@
         <v>1</v>
       </c>
       <c r="H124" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11">
       <c r="A125" t="s">
         <v>140</v>
       </c>
@@ -4361,7 +4445,7 @@
         <v>6</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D125">
         <v>96</v>
@@ -4376,10 +4460,10 @@
         <v>1</v>
       </c>
       <c r="H125" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="126" spans="1:8">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11">
       <c r="A126" t="s">
         <v>141</v>
       </c>
@@ -4387,7 +4471,7 @@
         <v>6</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D126">
         <v>96</v>
@@ -4402,10 +4486,10 @@
         <v>1</v>
       </c>
       <c r="H126" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11">
       <c r="A127" t="s">
         <v>130</v>
       </c>
@@ -4413,7 +4497,7 @@
         <v>6</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D127">
         <v>0</v>
@@ -4428,10 +4512,10 @@
         <v>1</v>
       </c>
       <c r="H127" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11">
       <c r="A128" t="s">
         <v>132</v>
       </c>
@@ -4439,7 +4523,7 @@
         <v>6</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D128">
         <v>24</v>
@@ -4454,7 +4538,7 @@
         <v>1</v>
       </c>
       <c r="H128" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="129" spans="1:8">
@@ -4465,7 +4549,7 @@
         <v>6</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D129">
         <v>3</v>
@@ -4480,7 +4564,7 @@
         <v>1</v>
       </c>
       <c r="H129" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="130" spans="1:8">
@@ -4491,7 +4575,7 @@
         <v>6</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D130">
         <v>48</v>
@@ -4506,7 +4590,7 @@
         <v>1</v>
       </c>
       <c r="H130" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="131" spans="1:8">
@@ -4517,7 +4601,7 @@
         <v>6</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D131">
         <v>72</v>
@@ -4532,7 +4616,7 @@
         <v>1</v>
       </c>
       <c r="H131" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="132" spans="1:8">
@@ -4543,13 +4627,13 @@
         <v>6</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D132">
         <v>96</v>
       </c>
       <c r="E132" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F132">
         <v>2</v>
@@ -4558,7 +4642,7 @@
         <v>1</v>
       </c>
       <c r="H132" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="133" spans="1:8">
@@ -4569,7 +4653,7 @@
         <v>7</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D133">
         <v>96</v>
@@ -4584,7 +4668,7 @@
         <v>1</v>
       </c>
       <c r="H133" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="134" spans="1:8">
@@ -4595,7 +4679,7 @@
         <v>7</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D134">
         <v>96</v>
@@ -4610,7 +4694,7 @@
         <v>1</v>
       </c>
       <c r="H134" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="135" spans="1:8">
@@ -4621,13 +4705,13 @@
         <v>7</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D135">
         <v>96</v>
       </c>
       <c r="E135" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F135">
         <v>2</v>
@@ -4636,7 +4720,7 @@
         <v>1</v>
       </c>
       <c r="H135" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="136" spans="1:8">
@@ -4647,7 +4731,7 @@
         <v>7</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D136">
         <v>0</v>
@@ -4662,7 +4746,7 @@
         <v>1</v>
       </c>
       <c r="H136" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="137" spans="1:8">
@@ -4673,7 +4757,7 @@
         <v>7</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D137">
         <v>24</v>
@@ -4688,7 +4772,7 @@
         <v>1</v>
       </c>
       <c r="H137" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="138" spans="1:8">
@@ -4699,7 +4783,7 @@
         <v>7</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D138">
         <v>3</v>
@@ -4714,7 +4798,7 @@
         <v>1</v>
       </c>
       <c r="H138" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="139" spans="1:8">
@@ -4725,7 +4809,7 @@
         <v>7</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D139">
         <v>48</v>
@@ -4740,7 +4824,7 @@
         <v>1</v>
       </c>
       <c r="H139" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="140" spans="1:8">
@@ -4751,7 +4835,7 @@
         <v>7</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D140">
         <v>48</v>
@@ -4766,7 +4850,7 @@
         <v>1</v>
       </c>
       <c r="H140" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="141" spans="1:8">
@@ -4777,7 +4861,7 @@
         <v>7</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D141">
         <v>72</v>
@@ -4792,7 +4876,7 @@
         <v>1</v>
       </c>
       <c r="H141" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="142" spans="1:8">
@@ -4803,7 +4887,7 @@
         <v>8</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D142">
         <v>96</v>
@@ -4818,7 +4902,7 @@
         <v>1</v>
       </c>
       <c r="H142" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="143" spans="1:8">
@@ -4829,7 +4913,7 @@
         <v>8</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D143">
         <v>96</v>
@@ -4844,7 +4928,7 @@
         <v>1</v>
       </c>
       <c r="H143" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="144" spans="1:8">
@@ -4855,13 +4939,13 @@
         <v>8</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D144">
         <v>96</v>
       </c>
       <c r="E144" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F144">
         <v>2</v>
@@ -4870,7 +4954,7 @@
         <v>1</v>
       </c>
       <c r="H144" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="145" spans="1:8">
@@ -4881,7 +4965,7 @@
         <v>8</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D145">
         <v>0</v>
@@ -4896,7 +4980,7 @@
         <v>1</v>
       </c>
       <c r="H145" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="146" spans="1:8">
@@ -4907,7 +4991,7 @@
         <v>8</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D146">
         <v>24</v>
@@ -4922,7 +5006,7 @@
         <v>1</v>
       </c>
       <c r="H146" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="147" spans="1:8">
@@ -4933,7 +5017,7 @@
         <v>8</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D147">
         <v>3</v>
@@ -4948,7 +5032,7 @@
         <v>1</v>
       </c>
       <c r="H147" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="148" spans="1:8">
@@ -4959,7 +5043,7 @@
         <v>8</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D148">
         <v>48</v>
@@ -4974,7 +5058,7 @@
         <v>1</v>
       </c>
       <c r="H148" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="149" spans="1:8">
@@ -4985,7 +5069,7 @@
         <v>8</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D149">
         <v>72</v>
@@ -5000,7 +5084,7 @@
         <v>1</v>
       </c>
       <c r="H149" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="150" spans="1:8">
@@ -5011,7 +5095,7 @@
         <v>9</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D150">
         <v>96</v>
@@ -5026,7 +5110,7 @@
         <v>1</v>
       </c>
       <c r="H150" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="151" spans="1:8">
@@ -5037,7 +5121,7 @@
         <v>9</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D151">
         <v>96</v>
@@ -5052,7 +5136,7 @@
         <v>1</v>
       </c>
       <c r="H151" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="152" spans="1:8">
@@ -5063,7 +5147,7 @@
         <v>9</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D152">
         <v>0</v>
@@ -5078,7 +5162,7 @@
         <v>1</v>
       </c>
       <c r="H152" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="153" spans="1:8">
@@ -5089,7 +5173,7 @@
         <v>9</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D153">
         <v>24</v>
@@ -5104,7 +5188,7 @@
         <v>1</v>
       </c>
       <c r="H153" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="154" spans="1:8">
@@ -5115,7 +5199,7 @@
         <v>9</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D154">
         <v>3</v>
@@ -5130,7 +5214,7 @@
         <v>1</v>
       </c>
       <c r="H154" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="155" spans="1:8">
@@ -5141,7 +5225,7 @@
         <v>9</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D155">
         <v>48</v>
@@ -5156,7 +5240,7 @@
         <v>1</v>
       </c>
       <c r="H155" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="156" spans="1:8">
@@ -5167,7 +5251,7 @@
         <v>9</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D156">
         <v>72</v>
@@ -5182,7 +5266,7 @@
         <v>1</v>
       </c>
       <c r="H156" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="157" spans="1:8">
@@ -5193,13 +5277,13 @@
         <v>9</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D157">
         <v>96</v>
       </c>
       <c r="E157" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F157">
         <v>2</v>
@@ -5208,7 +5292,7 @@
         <v>1</v>
       </c>
       <c r="H157" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="158" spans="1:8">
@@ -5219,7 +5303,7 @@
         <v>10</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D158">
         <v>96</v>
@@ -5234,7 +5318,7 @@
         <v>1</v>
       </c>
       <c r="H158" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="159" spans="1:8">
@@ -5245,7 +5329,7 @@
         <v>10</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D159">
         <v>96</v>
@@ -5260,7 +5344,7 @@
         <v>1</v>
       </c>
       <c r="H159" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="160" spans="1:8">
@@ -5271,7 +5355,7 @@
         <v>10</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D160">
         <v>24</v>
@@ -5286,7 +5370,7 @@
         <v>1</v>
       </c>
       <c r="H160" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="161" spans="1:8">
@@ -5297,7 +5381,7 @@
         <v>10</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D161">
         <v>3</v>
@@ -5312,7 +5396,7 @@
         <v>1</v>
       </c>
       <c r="H161" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="162" spans="1:8">
@@ -5323,13 +5407,13 @@
         <v>10</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D162">
         <v>96</v>
       </c>
       <c r="E162" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F162">
         <v>2</v>
@@ -5338,7 +5422,7 @@
         <v>1</v>
       </c>
       <c r="H162" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="163" spans="1:8">
@@ -5349,13 +5433,13 @@
         <v>10</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D163">
         <v>96</v>
       </c>
       <c r="E163" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F163">
         <v>2</v>
@@ -5364,7 +5448,7 @@
         <v>1</v>
       </c>
       <c r="H163" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="164" spans="1:8">
@@ -5375,7 +5459,7 @@
         <v>11</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D164">
         <v>0</v>
@@ -5390,7 +5474,7 @@
         <v>1</v>
       </c>
       <c r="H164" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="165" spans="1:8">
@@ -5401,7 +5485,7 @@
         <v>11</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D165">
         <v>3</v>
@@ -5416,7 +5500,7 @@
         <v>1</v>
       </c>
       <c r="H165" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="166" spans="1:8">
@@ -5427,7 +5511,7 @@
         <v>11</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D166">
         <v>3</v>
@@ -5442,7 +5526,7 @@
         <v>1</v>
       </c>
       <c r="H166" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="167" spans="1:8">
@@ -5453,13 +5537,13 @@
         <v>11</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D167">
         <v>3</v>
       </c>
       <c r="E167" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="F167">
         <v>2</v>
@@ -5468,7 +5552,7 @@
         <v>1</v>
       </c>
       <c r="H167" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="168" spans="1:8">
@@ -5479,7 +5563,7 @@
         <v>11</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D168">
         <v>3</v>
@@ -5494,7 +5578,7 @@
         <v>1</v>
       </c>
       <c r="H168" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="169" spans="1:8">
@@ -5505,7 +5589,7 @@
         <v>12</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D169">
         <v>96</v>
@@ -5520,7 +5604,7 @@
         <v>1</v>
       </c>
       <c r="H169" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="170" spans="1:8">
@@ -5531,7 +5615,7 @@
         <v>12</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D170">
         <v>96</v>
@@ -5546,7 +5630,7 @@
         <v>1</v>
       </c>
       <c r="H170" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="171" spans="1:8">
@@ -5557,7 +5641,7 @@
         <v>12</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D171">
         <v>0</v>
@@ -5572,7 +5656,7 @@
         <v>1</v>
       </c>
       <c r="H171" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="172" spans="1:8">
@@ -5583,7 +5667,7 @@
         <v>12</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D172">
         <v>24</v>
@@ -5598,7 +5682,7 @@
         <v>1</v>
       </c>
       <c r="H172" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="173" spans="1:8">
@@ -5609,7 +5693,7 @@
         <v>12</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D173">
         <v>3</v>
@@ -5624,7 +5708,7 @@
         <v>1</v>
       </c>
       <c r="H173" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="174" spans="1:8">
@@ -5635,13 +5719,13 @@
         <v>12</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D174">
         <v>96</v>
       </c>
       <c r="E174" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F174">
         <v>2</v>
@@ -5650,7 +5734,7 @@
         <v>1</v>
       </c>
       <c r="H174" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="175" spans="1:8">
@@ -5661,13 +5745,13 @@
         <v>12</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D175">
         <v>96</v>
       </c>
       <c r="E175" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F175">
         <v>2</v>
@@ -5676,7 +5760,7 @@
         <v>1</v>
       </c>
       <c r="H175" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="176" spans="1:8">
@@ -5687,7 +5771,7 @@
         <v>13</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="D176">
         <v>0</v>
@@ -5702,7 +5786,7 @@
         <v>1</v>
       </c>
       <c r="H176" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="177" spans="1:8">
@@ -5713,7 +5797,7 @@
         <v>13</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="D177">
         <v>3</v>
@@ -5728,7 +5812,7 @@
         <v>1</v>
       </c>
       <c r="H177" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="178" spans="1:8">
@@ -5739,7 +5823,7 @@
         <v>13</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="D178">
         <v>3</v>
@@ -5754,7 +5838,7 @@
         <v>1</v>
       </c>
       <c r="H178" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="179" spans="1:8">
@@ -5765,7 +5849,7 @@
         <v>13</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="D179">
         <v>3</v>
@@ -5780,7 +5864,7 @@
         <v>1</v>
       </c>
       <c r="H179" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="180" spans="1:8">
@@ -5791,13 +5875,13 @@
         <v>13</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="D180">
         <v>3</v>
       </c>
       <c r="E180" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F180">
         <v>2</v>
@@ -5806,7 +5890,7 @@
         <v>1</v>
       </c>
       <c r="H180" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="181" spans="1:8">
@@ -5817,13 +5901,13 @@
         <v>13</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="D181">
         <v>3</v>
       </c>
       <c r="E181" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="F181">
         <v>2</v>
@@ -5832,7 +5916,7 @@
         <v>1</v>
       </c>
       <c r="H181" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="182" spans="1:8">
@@ -5843,7 +5927,7 @@
         <v>14</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="D182">
         <v>0</v>
@@ -5858,7 +5942,7 @@
         <v>1</v>
       </c>
       <c r="H182" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="183" spans="1:8">
@@ -5869,7 +5953,7 @@
         <v>14</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="D183">
         <v>24</v>
@@ -5884,7 +5968,7 @@
         <v>1</v>
       </c>
       <c r="H183" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="184" spans="1:8">
@@ -5895,7 +5979,7 @@
         <v>14</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="D184">
         <v>48</v>
@@ -5910,7 +5994,7 @@
         <v>1</v>
       </c>
       <c r="H184" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="185" spans="1:8">
@@ -5921,7 +6005,7 @@
         <v>14</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="D185">
         <v>48</v>
@@ -5936,7 +6020,7 @@
         <v>1</v>
       </c>
       <c r="H185" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="186" spans="1:8">
@@ -5947,7 +6031,7 @@
         <v>14</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="D186">
         <v>48</v>
@@ -5962,7 +6046,7 @@
         <v>1</v>
       </c>
       <c r="H186" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="187" spans="1:8">
@@ -5973,7 +6057,7 @@
         <v>14</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="D187">
         <v>48</v>
@@ -5988,7 +6072,7 @@
         <v>1</v>
       </c>
       <c r="H187" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="193" spans="1:6">
@@ -5996,7 +6080,7 @@
         <v>186</v>
       </c>
       <c r="B193" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D193">
         <v>72</v>

</xml_diff>